<commit_message>
Final - Perception not working
Relatorio Acabado
Resto dos testes feitos
</commit_message>
<xml_diff>
--- a/food-cells.xlsx
+++ b/food-cells.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Virgilio\OneDrive\ISEC\Ano 2\1º Semestre\I.I.A\IIA---TP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DA1131-4A00-4872-9A05-CBC9B4B56C0D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -692,7 +692,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -765,7 +765,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -930,7 +930,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -968,7 +968,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1629896784"/>
@@ -1027,7 +1027,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1627327744"/>
@@ -1068,7 +1068,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1986,17 +1986,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="G343" sqref="G343"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" customWidth="1"/>
+    <col min="6" max="6" width="20.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>5</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>5</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>5</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>5</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>5</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>5</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>5</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>5</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>5</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>5</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>5</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>5</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>5</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>5</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>5</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>5</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>5</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>5</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>5</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>5</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>5</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>5</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>5</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>5</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>5</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>5</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>5</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>5</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>5</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>5</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>5</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>5</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>5</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>5</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>5</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>5</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>5</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>5</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>5</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>5</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>5</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>5</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>5</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>5</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>5</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>5</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>5</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>5</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>5</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>5</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>5</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>5</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>5</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>5</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>5</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>5</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>5</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>5</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>5</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>5</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>10</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>5</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>5</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>10</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>10</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>10</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>10</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>10</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>10</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>10</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>10</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>10</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>10</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>10</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>10</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>10</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>10</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>10</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>10</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>10</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>10</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>10</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>10</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>10</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>10</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>10</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>10</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>10</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>10</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>10</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>10</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>10</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>10</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>10</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>10</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>10</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>10</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>10</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>10</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>10</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>10</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>10</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>10</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>10</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>10</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>10</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>10</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>10</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>10</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>10</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>10</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>10</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>10</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>10</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>10</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>10</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>10</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>10</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>10</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>10</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>10</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>10</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>10</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>10</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>10</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>10</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>10</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>10</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>10</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>10</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>10</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>10</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>10</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>10</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>10</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>10</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>10</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>10</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>10</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>10</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>10</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>10</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>10</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>10</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>10</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>10</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>10</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>10</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>10</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>10</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>10</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>10</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>10</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>10</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>10</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>10</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>10</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>10</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>10</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>10</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>10</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>10</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>15</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>15</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>15</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>15</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>15</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>15</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>15</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>15</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>15</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>15</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>15</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>15</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>15</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>15</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>15</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>15</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>15</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>15</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>15</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>15</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>15</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>15</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>15</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>15</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>15</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>15</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>15</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>15</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>15</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>15</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>15</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>15</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>15</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>15</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>15</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>15</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>15</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>15</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>15</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>15</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>15</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>15</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>15</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>15</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>15</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>15</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>15</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>15</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>15</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>15</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>15</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>15</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>15</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>15</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>15</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>15</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>15</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>15</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>15</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>15</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>15</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>15</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>15</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>15</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>15</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>15</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>15</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A268">
         <v>15</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A269">
         <v>15</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A270">
         <v>15</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A271">
         <v>15</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A272">
         <v>15</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A273">
         <v>15</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>15</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A275">
         <v>15</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>15</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>15</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>15</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>15</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>15</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A281">
         <v>15</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A282">
         <v>15</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A283">
         <v>15</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A284">
         <v>15</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A285">
         <v>15</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A286">
         <v>15</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A287">
         <v>15</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A288">
         <v>15</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A289">
         <v>15</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A290">
         <v>15</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A291">
         <v>15</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A292">
         <v>15</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A293">
         <v>15</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A294">
         <v>15</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A295">
         <v>15</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A296">
         <v>15</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A297">
         <v>15</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A298">
         <v>15</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A299">
         <v>20</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A300">
         <v>15</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A301">
         <v>15</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A302">
         <v>20</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A303">
         <v>20</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A304">
         <v>20</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A305">
         <v>20</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A306">
         <v>20</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A307">
         <v>20</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A308">
         <v>20</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A309">
         <v>20</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A310">
         <v>20</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A311">
         <v>20</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A312">
         <v>20</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A313">
         <v>20</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A314">
         <v>20</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A315">
         <v>20</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A316">
         <v>20</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A317">
         <v>20</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A318">
         <v>20</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A319">
         <v>20</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A320">
         <v>20</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A321">
         <v>20</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A322">
         <v>20</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A323">
         <v>20</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>20</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>20</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>20</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>20</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>20</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>20</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>20</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A331">
         <v>20</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A332">
         <v>20</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A333">
         <v>20</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A334">
         <v>20</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A335">
         <v>20</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A336">
         <v>20</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A337">
         <v>20</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A338">
         <v>20</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A339">
         <v>20</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>20</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>20</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A342">
         <v>20</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A343">
         <v>20</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A344">
         <v>20</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A345">
         <v>20</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A346">
         <v>20</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A347">
         <v>20</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A348">
         <v>20</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A349">
         <v>20</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A350">
         <v>20</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A351">
         <v>20</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A352">
         <v>20</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A353">
         <v>20</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A354">
         <v>20</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A355">
         <v>20</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A356">
         <v>20</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A357">
         <v>20</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A358">
         <v>20</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A359">
         <v>20</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A360">
         <v>20</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A361">
         <v>20</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A362">
         <v>20</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A363">
         <v>20</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A364">
         <v>20</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A365">
         <v>20</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A366">
         <v>20</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A367">
         <v>20</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A368">
         <v>20</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A369">
         <v>20</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A370">
         <v>20</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A371">
         <v>20</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A372">
         <v>20</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A373">
         <v>20</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A374">
         <v>20</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A375">
         <v>20</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A376">
         <v>20</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A377">
         <v>20</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A378">
         <v>20</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A379">
         <v>20</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A380">
         <v>20</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A381">
         <v>20</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A382">
         <v>20</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A383">
         <v>20</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A384">
         <v>20</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A385">
         <v>20</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A386">
         <v>20</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A387">
         <v>20</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A388">
         <v>20</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A389">
         <v>20</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A390">
         <v>20</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A391">
         <v>20</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A392">
         <v>20</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A393">
         <v>20</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A394">
         <v>20</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A395">
         <v>20</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A396">
         <v>20</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A397">
         <v>20</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A398">
         <v>20</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A399">
         <v>20</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A400">
         <v>20</v>
       </c>

</xml_diff>